<commit_message>
according to board: pho-klite, change the pinout
</commit_message>
<xml_diff>
--- a/DOC/pin分配.xlsx
+++ b/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PB1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PH2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,7 +96,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一体板光敏电阻输入,ADC12_IN9</t>
+    <t>输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beeper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外部光敏电阻输入,ADC12_IN4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -482,7 +502,8 @@
     <col min="1" max="1" width="12.1328125" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.73046875" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.3984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="1"/>
+    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -539,22 +560,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -563,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -571,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -580,7 +603,24 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>